<commit_message>
create acid_dissociation_constants and updated chemicals and institutions
</commit_message>
<xml_diff>
--- a/micropol_template.xlsx
+++ b/micropol_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="995" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="995" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Chemical" sheetId="1" state="visible" r:id="rId2"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="105">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -202,82 +202,109 @@
     <t xml:space="preserve">identifier</t>
   </si>
   <si>
-    <t xml:space="preserve">is_representative</t>
+    <t xml:space="preserve">perfluoroheptanoicacid_0_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">perfluoroheptanoicacid_-1_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hypychlorous acid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hypychlorousacid_0_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hypychlorousacid_-1_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-methyl-1h-benzotriazole_0_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-methyl-1h-benzotriazole_-1_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-methyl-1h-benzotriazole_-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">is_experimental</t>
+  </si>
+  <si>
+    <t xml:space="preserve">temperature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ph</t>
+  </si>
+  <si>
+    <t xml:space="preserve">doi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">url</t>
   </si>
   <si>
     <t xml:space="preserve">perfluoroheptanoicacid0a</t>
   </si>
   <si>
+    <t xml:space="preserve">experimental_or_predicted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">elementary_or_apparent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wavelength</t>
+  </si>
+  <si>
+    <t xml:space="preserve">experimental</t>
+  </si>
+  <si>
+    <t xml:space="preserve">apparent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reactant1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reactant2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hypychlorousacid0a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hypychlorousacid-1a</t>
+  </si>
+  <si>
     <t xml:space="preserve">perfluoroheptanoicacid-1a</t>
   </si>
   <si>
-    <t xml:space="preserve">hypychlorous acid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hypychlorousacid0a</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hypychlorousacid-1a</t>
-  </si>
-  <si>
     <t xml:space="preserve">4methyl1hbenzotriazole0a</t>
   </si>
   <si>
     <t xml:space="preserve">4methyl1hbenzotriazole-1a</t>
   </si>
   <si>
-    <t xml:space="preserve">value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">is_experimental</t>
-  </si>
-  <si>
-    <t xml:space="preserve">temperature</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ph</t>
-  </si>
-  <si>
-    <t xml:space="preserve">doi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">url</t>
-  </si>
-  <si>
-    <t xml:space="preserve">experimental_or_predicted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">elementary_or_apparent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wavelength</t>
-  </si>
-  <si>
-    <t xml:space="preserve">experimental</t>
-  </si>
-  <si>
-    <t xml:space="preserve">apparent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reactant1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reactant2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">unit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hypychlorousacid-1a</t>
-  </si>
-  <si>
     <t xml:space="preserve">uv254nm[model][company]</t>
   </si>
   <si>
-    <t xml:space="preserve">acid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">conjugate_base</t>
+    <t xml:space="preserve">branching_ratio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Perfluoroheptanoicacid_0_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hypychlorousacid_0_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4methyl1hbenzotriazole_0_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4methyl1hbenzotriazole_-1_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4methyl1hbenzotriazole_-1_2</t>
   </si>
   <si>
     <t xml:space="preserve">medium</t>
@@ -413,7 +440,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -438,6 +465,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -457,19 +488,19 @@
   </sheetPr>
   <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="59.8469387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="47.8775510204082"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="19.8010204081633"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="15.8367346938776"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="16.8265306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="1" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="64.1683673469388"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.780612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="51.2959183673469"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="21.2397959183673"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="16.9183673469388"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="17.9081632653061"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="1" width="12.780612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -763,34 +794,34 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.8265306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.91836734693878"/>
-    <col collapsed="false" hidden="false" max="6" min="3" style="0" width="6.01020408163265"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="32.7295918367347"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="3.73469387755102"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="3.37244897959184"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="71.9030612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.35714285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="6" min="3" style="0" width="6.38775510204082"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="35.0102040816326"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="3.86734693877551"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="3.51020408163265"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="77.2142857142857"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="12.3316326530612"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>56</v>
@@ -807,34 +838,34 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="5"/>
       <c r="G2" s="1" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -856,15 +887,15 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.9285714285714"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.7397959183673"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.6377551020408"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.780612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="12.780612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1082,20 +1113,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.3979591836735"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.219387755102"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.1887755102041"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.0204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.0051020408163"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="12.780612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1112,9 +1142,6 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="F1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1126,11 +1153,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E2" s="5" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1141,47 +1164,34 @@
         <v>-1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E3" s="5" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
-      <c r="E4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>0</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E5" s="5" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B6" s="1" t="n">
         <v>-1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E6" s="5" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1197,7 +1207,7 @@
         <v>0</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1208,6 +1218,17 @@
         <v>-1</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1235,10 +1256,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.0612244897959"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.4897959183673"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.5867346938776"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.780612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="12.780612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1269,7 +1290,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>3.2</v>
@@ -1310,11 +1331,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.0612244897959"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.4897959183673"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.1836734693878"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.5867346938776"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.780612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="12.780612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1345,7 +1366,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>3.2</v>
@@ -1388,11 +1409,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.8214285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.1938775510204"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.1836734693878"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.3061224489796"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.780612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.75"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="12.780612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1403,13 +1424,13 @@
         <v>65</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>67</v>
@@ -1429,16 +1450,16 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>3000</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E2" s="1" t="n">
         <v>254</v>
@@ -1474,11 +1495,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.0612244897959"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.8214285714286"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.1836734693878"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.5867346938776"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.780612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.3877551020408"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="12.780612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1489,13 +1510,13 @@
         <v>65</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>67</v>
@@ -1562,32 +1583,32 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="31.0459183673469"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="44.9948979591837"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="1" width="22.8214285714286"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="21.1836734693878"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="33.2091836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="48.3265306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.780612244898"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="1" width="24.3877551020408"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="12.780612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>65</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>67</v>
@@ -1607,10 +1628,10 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="1" t="n">
@@ -1619,16 +1640,19 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>79</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="E3" s="0"/>
+      <c r="F3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>59</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="B4" s="0"/>
       <c r="E4" s="5"/>
       <c r="F4" s="1" t="n">
         <v>25</v>
@@ -1636,42 +1660,46 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>63</v>
+        <v>83</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>63</v>
+        <v>83</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>64</v>
+        <v>84</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>64</v>
+        <v>84</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>79</v>
-      </c>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0"/>
+      <c r="B9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>64</v>
+        <v>84</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1690,77 +1718,126 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.0459183673469"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="44.9948979591837"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.8214285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.2091836734694"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="12.780612244898"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="24.3877551020408"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="12.780612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>81</v>
+        <v>56</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>82</v>
+        <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>65</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>71</v>
+        <v>86</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>59</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="1" t="n">
+      <c r="D2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" s="5"/>
+      <c r="F2" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>79</v>
-      </c>
+        <v>88</v>
+      </c>
+      <c r="B3" s="1"/>
       <c r="C3" s="1" t="n">
         <v>7.5</v>
       </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="1" t="n">
+      <c r="D3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" s="5"/>
+      <c r="F3" s="1" t="n">
         <v>25</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="D4" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" s="6" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="6" t="n">
+        <v>8.6</v>
+      </c>
+      <c r="D5" s="6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F5" s="6" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="6" t="n">
+        <v>8.6</v>
+      </c>
+      <c r="D6" s="6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F6" s="6" t="n">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>